<commit_message>
revised entire collection: Split compilation games into distinct entries Added columns to tables to: look into value for money, based on hours played (as well as the paid price) noting various dates in relation to all games present.
</commit_message>
<xml_diff>
--- a/playstation/output/finances_average_totals.xlsx
+++ b/playstation/output/finances_average_totals.xlsx
@@ -335,16 +335,16 @@
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>943.0</v>
+        <v>1035.0</v>
       </c>
       <c r="B2" s="3">
-        <v>24.1989</v>
+        <v>23.9532</v>
       </c>
       <c r="C2" s="3">
-        <v>10.822</v>
+        <v>10.2435</v>
       </c>
       <c r="D2" s="3">
-        <v>13.3769</v>
+        <v>13.7097</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>

</xml_diff>